<commit_message>
zip ++ color =+
</commit_message>
<xml_diff>
--- a/colors.xlsx
+++ b/colors.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waok2hurricane/Desktop/lazima/projects/play-area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930303C0-46D5-924A-9EDD-0990F0560169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E686745D-E83B-994E-8E21-FA425148A8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{33E7EB2D-2B52-BB4B-A71E-BD1F0E428788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,12 +35,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Red</t>
   </si>
   <si>
-    <t>blue</t>
+    <t xml:space="preserve">orange </t>
+  </si>
+  <si>
+    <t>blue -1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new sheet </t>
   </si>
 </sst>
 </file>
@@ -391,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D2C004-123D-A14C-B3B9-505451C22602}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -406,10 +413,33 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA935B9-1328-534D-B86E-D13EEFC0A42A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>